<commit_message>
Added buttons without using xlsxwriter, and fixed rows and requirements.txt
</commit_message>
<xml_diff>
--- a/dist/My Movie Library.xlsx
+++ b/dist/My Movie Library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\TMDBScrappers\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8FF129-549C-41EE-A580-7DE41D10131E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEECFDD9-F810-4ED9-8B61-38CE0EEFD8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4824" yWindow="2160" windowWidth="17280" windowHeight="9228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="9228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,11 +479,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A3:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,37 +492,37 @@
     <col min="7" max="7" width="46.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>